<commit_message>
DPF et plan de test fixés, routine mise à jour.
</commit_message>
<xml_diff>
--- a/Remises/Remise 2/DPF.xlsx
+++ b/Remises/Remise 2/DPF.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles-Olivier\Documents\design3\Remises\Remise 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles-Olivier\Documents\Ulaval\Hiver 2016\Remises\Remise 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="8025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="8030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="107">
   <si>
     <t>Naviguer autour des îles</t>
   </si>
   <si>
-    <t>Lire la tension aux bornes du condensateur</t>
-  </si>
-  <si>
     <t>Éviter contact avec les murs</t>
   </si>
   <si>
@@ -77,21 +74,12 @@
     <t>Soulever un trésor</t>
   </si>
   <si>
-    <t>de façon autonome</t>
-  </si>
-  <si>
     <t>système</t>
   </si>
   <si>
     <t>Communiquer entre les éléments du</t>
   </si>
   <si>
-    <t>Gérer le condensateur</t>
-  </si>
-  <si>
-    <t>Affichage de la tension du condensateur et de la trajectoire planifiée, de la position et de l'orientation du robot  en temps réel sur la station de base</t>
-  </si>
-  <si>
     <t>Activer la routine au démarrage du micro-PC sans requête extérieure</t>
   </si>
   <si>
@@ -131,30 +119,18 @@
     <t>Tension min (V)</t>
   </si>
   <si>
-    <t>Tension max (V)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Alimenter le robot avec </t>
   </si>
   <si>
     <t>une batterie unique</t>
   </si>
   <si>
-    <t>une tension précise</t>
-  </si>
-  <si>
-    <t>Charger le condensateur jusqu'à</t>
-  </si>
-  <si>
     <t>cas de danger</t>
   </si>
   <si>
     <t>Signaler une alerte en</t>
   </si>
   <si>
-    <t>Temps avant affichage (s)</t>
-  </si>
-  <si>
     <t>composantes internes</t>
   </si>
   <si>
@@ -179,18 +155,12 @@
     <t>Afficher les trajectoires (prévue et réelle)</t>
   </si>
   <si>
-    <t>Taux de rafraîchissage (Hz)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Communiquer entre l'ordinateur du robot </t>
   </si>
   <si>
     <t>et le microcontrôlleur par UART</t>
   </si>
   <si>
-    <t>délai (ms)</t>
-  </si>
-  <si>
     <t>Interpréter une vision</t>
   </si>
   <si>
@@ -203,33 +173,15 @@
     <t>Précision du temps écoulé (s)</t>
   </si>
   <si>
-    <t>Précision (cm)</t>
-  </si>
-  <si>
     <t>Distinguer les trésors</t>
   </si>
   <si>
-    <t>Temps de charge (s)</t>
-  </si>
-  <si>
-    <t>Précision (V)</t>
-  </si>
-  <si>
-    <t>Ramasser un trésor à l'aide</t>
-  </si>
-  <si>
     <t>d'un préhenseur</t>
   </si>
   <si>
-    <t>Durée maximale du régime transitoire (s)</t>
-  </si>
-  <si>
     <t>Commander les roues du robot</t>
   </si>
   <si>
-    <t>Précision de l'asservissement (%)</t>
-  </si>
-  <si>
     <t>Durée de rotation (s)</t>
   </si>
   <si>
@@ -239,9 +191,6 @@
     <t>Poids maximal soulevé (g)</t>
   </si>
   <si>
-    <t>Temps de saisie (s)</t>
-  </si>
-  <si>
     <t>Temps avant décharge (s)</t>
   </si>
   <si>
@@ -257,12 +206,6 @@
     <t xml:space="preserve"> à partir de la station</t>
   </si>
   <si>
-    <t>Recevoir la charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> par induction</t>
-  </si>
-  <si>
     <t>Afficher la position et</t>
   </si>
   <si>
@@ -275,15 +218,6 @@
     <t xml:space="preserve"> et des cellules de la batterie</t>
   </si>
   <si>
-    <t xml:space="preserve">Afficher la forme ou la couleur </t>
-  </si>
-  <si>
-    <t>de l'île cible sur la station de base</t>
-  </si>
-  <si>
-    <t>Vitesse de transmission (bps)</t>
-  </si>
-  <si>
     <t>Communiquer sans fil entre l'ordinateur</t>
   </si>
   <si>
@@ -299,15 +233,6 @@
     <t>du robot et le serveur d'îles</t>
   </si>
   <si>
-    <t>Reconnaître les formes</t>
-  </si>
-  <si>
-    <t>Détecter un décalage par rapport</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> à la station de recharge</t>
-  </si>
-  <si>
     <t>Alimenter tous les éléments du robot de manière autonome</t>
   </si>
   <si>
@@ -323,13 +248,103 @@
     <t>Fréquence de mise à jour de la trajectoire (Hz)</t>
   </si>
   <si>
-    <t>Vitesse (rad/s)</t>
-  </si>
-  <si>
     <t>Tourner la</t>
   </si>
   <si>
-    <t xml:space="preserve"> des îles et du robot</t>
+    <t>Variation de tension des régulateurs (V)</t>
+  </si>
+  <si>
+    <t>Temps de recharge (s)</t>
+  </si>
+  <si>
+    <t>Charger le condensateur jusqu'à une tension précise</t>
+  </si>
+  <si>
+    <t>Temps avant alarme (s)</t>
+  </si>
+  <si>
+    <t>Courant max (A)</t>
+  </si>
+  <si>
+    <t>Exècuter une routine complète</t>
+  </si>
+  <si>
+    <t>en moins de 10 minutes</t>
+  </si>
+  <si>
+    <t>Temps d'exécution (s)</t>
+  </si>
+  <si>
+    <t>Précision de la forme(cm)</t>
+  </si>
+  <si>
+    <t>Précision de la position (cm)</t>
+  </si>
+  <si>
+    <t>Reconnaître les îles</t>
+  </si>
+  <si>
+    <t>Reconnaître le robot</t>
+  </si>
+  <si>
+    <t>Affichage de la tension du condensateur et de la trajectoire planifiée, de la position et de l'orientation du robot en temps réel sur la station de base</t>
+  </si>
+  <si>
+    <t>S'enligner sur la station de</t>
+  </si>
+  <si>
+    <t>recharge</t>
+  </si>
+  <si>
+    <t>Précision sur la position</t>
+  </si>
+  <si>
+    <t>Déplacement minimal (cm)</t>
+  </si>
+  <si>
+    <t>Pourcentage de déviation (%)</t>
+  </si>
+  <si>
+    <t>Distance de freinage (cm)</t>
+  </si>
+  <si>
+    <t>Éviter les contacts avec les murs</t>
+  </si>
+  <si>
+    <t>et les îles</t>
+  </si>
+  <si>
+    <t>Précision du dépot (cm)</t>
+  </si>
+  <si>
+    <t>Maniupler un trésor à l'aide</t>
+  </si>
+  <si>
+    <t>du robot sur la station de base</t>
+  </si>
+  <si>
+    <t>Taux de rafraîchissement (Hz)</t>
+  </si>
+  <si>
+    <t>Précision de la lecture de tension</t>
+  </si>
+  <si>
+    <t>Affichage des îles et trésors</t>
+  </si>
+  <si>
+    <t>Délai maximal (ms)</t>
+  </si>
+  <si>
+    <t>Taux de réussite (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Décoder et envoyer la bonne lettre au </t>
+  </si>
+  <si>
+    <t>serveur des îles</t>
+  </si>
+  <si>
+    <t>Taux de réussite du décodage (%)</t>
   </si>
 </sst>
 </file>
@@ -353,7 +368,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -388,15 +403,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -511,11 +517,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" textRotation="90"/>
@@ -528,95 +556,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -901,385 +935,408 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD45"/>
+  <dimension ref="A1:AG45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC16" sqref="AC16"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AG13" sqref="AG13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="139.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
-    <col min="12" max="12" width="32" customWidth="1"/>
-    <col min="13" max="13" width="45.42578125" customWidth="1"/>
-    <col min="14" max="14" width="39.5703125" customWidth="1"/>
-    <col min="15" max="15" width="39.7109375" customWidth="1"/>
-    <col min="16" max="16" width="34.140625" customWidth="1"/>
-    <col min="17" max="17" width="26.85546875" customWidth="1"/>
-    <col min="18" max="18" width="31.85546875" customWidth="1"/>
-    <col min="19" max="19" width="26.5703125" customWidth="1"/>
-    <col min="20" max="20" width="27.85546875" customWidth="1"/>
-    <col min="21" max="21" width="23.140625" customWidth="1"/>
-    <col min="22" max="22" width="40.7109375" customWidth="1"/>
-    <col min="23" max="23" width="38.85546875" customWidth="1"/>
-    <col min="24" max="24" width="44.7109375" customWidth="1"/>
-    <col min="25" max="25" width="47.28515625" customWidth="1"/>
-    <col min="26" max="26" width="40.5703125" customWidth="1"/>
-    <col min="27" max="27" width="41" customWidth="1"/>
-    <col min="28" max="28" width="39" customWidth="1"/>
-    <col min="29" max="29" width="40.28515625" customWidth="1"/>
-    <col min="30" max="30" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="137" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="3" max="4" width="37.6328125" customWidth="1"/>
+    <col min="5" max="5" width="32.26953125" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" customWidth="1"/>
+    <col min="8" max="8" width="30.26953125" customWidth="1"/>
+    <col min="9" max="9" width="31.90625" customWidth="1"/>
+    <col min="10" max="10" width="33.26953125" customWidth="1"/>
+    <col min="11" max="11" width="36.7265625" customWidth="1"/>
+    <col min="12" max="12" width="25.90625" customWidth="1"/>
+    <col min="13" max="13" width="25.7265625" customWidth="1"/>
+    <col min="14" max="14" width="29.1796875" customWidth="1"/>
+    <col min="15" max="15" width="32" customWidth="1"/>
+    <col min="16" max="16" width="45.453125" customWidth="1"/>
+    <col min="17" max="17" width="39.54296875" customWidth="1"/>
+    <col min="18" max="18" width="39.7265625" customWidth="1"/>
+    <col min="19" max="19" width="34.1796875" customWidth="1"/>
+    <col min="20" max="20" width="26.81640625" customWidth="1"/>
+    <col min="21" max="21" width="31.81640625" customWidth="1"/>
+    <col min="22" max="22" width="26.54296875" customWidth="1"/>
+    <col min="23" max="23" width="27.81640625" customWidth="1"/>
+    <col min="24" max="24" width="40.54296875" customWidth="1"/>
+    <col min="25" max="26" width="30" customWidth="1"/>
+    <col min="27" max="27" width="47.7265625" customWidth="1"/>
+    <col min="28" max="28" width="37" customWidth="1"/>
+    <col min="29" max="29" width="47.26953125" customWidth="1"/>
+    <col min="30" max="30" width="40.54296875" customWidth="1"/>
+    <col min="31" max="31" width="41" customWidth="1"/>
+    <col min="32" max="32" width="39" customWidth="1"/>
+    <col min="33" max="33" width="40.26953125" customWidth="1"/>
+    <col min="34" max="34" width="40.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="B1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="V1" s="19"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="20"/>
+    </row>
+    <row r="2" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="22"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="23"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="37"/>
+      <c r="F3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="31"/>
+      <c r="S3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="U3" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="V3" s="25"/>
+      <c r="W3" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z3" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA3" s="35"/>
+      <c r="AB3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG3" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="B4" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="17" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4" s="26"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z4" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="W5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="S1" s="18"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="19"/>
-      <c r="W1" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="19"/>
-    </row>
-    <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="V2" s="29"/>
-      <c r="W2" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="29"/>
-      <c r="AA2" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="29"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="N3" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="8" t="s">
+      <c r="X5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z5" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="R3" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="T3" s="33"/>
-      <c r="U3" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="V3" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="W3" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="X3" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y3" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z3" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA3" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB3" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC3" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD3" s="31" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="N4" s="14"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="R4" s="13"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="V4" s="10"/>
-      <c r="W4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB4" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC4" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD4" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="M5" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="N5" s="7" t="s">
+      <c r="AA5" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="O5" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="V5" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="W5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="X5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA5" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="AB5" s="7" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="AC5" s="7" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="AD5" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="AE5" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF5" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG5" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1292,26 +1349,28 @@
       <c r="J6" s="2">
         <v>5</v>
       </c>
-      <c r="K6" s="2">
-        <v>5</v>
-      </c>
+      <c r="K6" s="2"/>
       <c r="L6" s="2">
-        <v>2</v>
-      </c>
-      <c r="M6" s="4">
-        <v>5</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="M6" s="2">
+        <v>5</v>
+      </c>
+      <c r="N6" s="2">
+        <v>5</v>
+      </c>
+      <c r="O6" s="2">
+        <v>3</v>
+      </c>
+      <c r="P6" s="4">
+        <v>5</v>
+      </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
-      <c r="V6" s="2">
-        <v>3</v>
-      </c>
+      <c r="V6" s="2"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
@@ -1320,10 +1379,13 @@
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -1343,7 +1405,9 @@
       <c r="G7" s="2">
         <v>5</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1353,18 +1417,14 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="2">
-        <v>5</v>
-      </c>
+      <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
-      <c r="U7" s="2">
-        <v>4</v>
-      </c>
-      <c r="V7" s="2">
-        <v>5</v>
-      </c>
-      <c r="W7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2">
+        <v>5</v>
+      </c>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
@@ -1372,8 +1432,11 @@
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1389,43 +1452,50 @@
         <v>5</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2">
-        <v>5</v>
-      </c>
+      <c r="L8" s="2">
+        <v>5</v>
+      </c>
+      <c r="M8" s="2"/>
       <c r="N8" s="2">
+        <v>5</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="2">
         <v>4</v>
       </c>
-      <c r="O8" s="2">
+      <c r="R8" s="2">
         <v>4</v>
       </c>
-      <c r="P8" s="2">
-        <v>5</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>3</v>
-      </c>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="S8" s="2">
+        <v>5</v>
+      </c>
+      <c r="T8" s="2">
+        <v>3</v>
+      </c>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
-      <c r="AA8" s="2">
-        <v>3</v>
-      </c>
-      <c r="AB8" s="2">
-        <v>5</v>
-      </c>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1439,55 +1509,60 @@
         <v>5</v>
       </c>
       <c r="K9" s="2"/>
-      <c r="L9" s="2">
-        <v>3</v>
-      </c>
-      <c r="M9" s="2">
-        <v>5</v>
-      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
       <c r="N9" s="2">
+        <v>5</v>
+      </c>
+      <c r="O9" s="2">
+        <v>3</v>
+      </c>
+      <c r="P9" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="2">
         <v>4</v>
       </c>
-      <c r="O9" s="2">
+      <c r="R9" s="2">
         <v>4</v>
       </c>
-      <c r="P9" s="2">
-        <v>5</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>3</v>
-      </c>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
+      <c r="S9" s="2">
+        <v>5</v>
+      </c>
+      <c r="T9" s="2">
+        <v>3</v>
+      </c>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
-      <c r="AA9" s="2">
-        <v>3</v>
-      </c>
-      <c r="AB9" s="2">
-        <v>5</v>
-      </c>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -1510,10 +1585,13 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1523,14 +1601,15 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2">
+        <v>5</v>
+      </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="2">
-        <v>5</v>
-      </c>
+      <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="O11" s="2">
+        <v>5</v>
+      </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -1543,17 +1622,20 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
-      <c r="AB11" s="2">
-        <v>5</v>
-      </c>
-      <c r="AC11" s="2">
-        <v>5</v>
-      </c>
-      <c r="AD11" s="2"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1563,7 +1645,9 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1584,10 +1668,15 @@
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1595,32 +1684,32 @@
         <v>5</v>
       </c>
       <c r="E13" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="J13" s="2">
+        <v>5</v>
+      </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="2">
-        <v>5</v>
-      </c>
+      <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
+      <c r="O13" s="2">
+        <v>5</v>
+      </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-      <c r="R13" s="2">
-        <v>5</v>
-      </c>
+      <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
-      <c r="V13" s="2">
-        <v>5</v>
-      </c>
-      <c r="W13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2">
+        <v>5</v>
+      </c>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
@@ -1628,17 +1717,22 @@
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2">
         <v>5</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1651,14 +1745,14 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="2">
-        <v>5</v>
-      </c>
+      <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
+      <c r="W14" s="2">
+        <v>5</v>
+      </c>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
@@ -1666,10 +1760,13 @@
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1679,23 +1776,29 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2">
-        <v>5</v>
-      </c>
+      <c r="J15" s="2">
+        <v>5</v>
+      </c>
+      <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="M15" s="2">
+        <v>5</v>
+      </c>
+      <c r="N15" s="2">
+        <v>5</v>
+      </c>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
-      <c r="T15" s="2">
-        <v>5</v>
-      </c>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2">
+        <v>5</v>
+      </c>
+      <c r="V15" s="2">
+        <v>5</v>
+      </c>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
@@ -1704,10 +1807,13 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1721,9 +1827,13 @@
         <v>5</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="L16" s="2">
+        <v>5</v>
+      </c>
       <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+      <c r="N16" s="2">
+        <v>5</v>
+      </c>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -1740,10 +1850,13 @@
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1753,59 +1866,62 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2">
-        <v>2</v>
-      </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="2">
         <v>2</v>
       </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="J17" s="2">
+        <v>5</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2</v>
+      </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="2">
-        <v>5</v>
-      </c>
-      <c r="O17" s="2">
-        <v>4</v>
-      </c>
-      <c r="P17" s="2">
-        <v>3</v>
-      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
       <c r="Q17" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R17" s="2">
         <v>4</v>
       </c>
       <c r="S17" s="2">
+        <v>3</v>
+      </c>
+      <c r="T17" s="2">
         <v>2</v>
       </c>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2">
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2">
         <v>4</v>
       </c>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
-      <c r="AA17" s="2">
-        <v>2</v>
-      </c>
-      <c r="AB17" s="2">
-        <v>2</v>
-      </c>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
       <c r="AC17" s="2">
         <v>2</v>
       </c>
       <c r="AD17" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE17" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF17" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG17" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1813,14 +1929,16 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2">
-        <v>5</v>
-      </c>
+      <c r="H18" s="2"/>
       <c r="I18" s="2">
         <v>5</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="J18" s="2">
+        <v>5</v>
+      </c>
+      <c r="K18" s="2">
+        <v>5</v>
+      </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1840,10 +1958,13 @@
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2">
         <v>3</v>
@@ -1852,13 +1973,13 @@
         <v>3</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="2">
-        <v>3</v>
-      </c>
+      <c r="E19" s="2"/>
       <c r="F19" s="2">
-        <v>5</v>
-      </c>
-      <c r="G19" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="G19" s="2">
+        <v>5</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1882,10 +2003,13 @@
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1916,10 +2040,13 @@
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" s="2">
         <v>4</v>
@@ -1931,12 +2058,14 @@
         <v>2</v>
       </c>
       <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2">
         <v>1</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>2</v>
       </c>
-      <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1956,22 +2085,25 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
-      <c r="AA21" s="2">
-        <v>3</v>
-      </c>
-      <c r="AB21" s="2">
-        <v>3</v>
-      </c>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
       <c r="AC21" s="2">
         <v>3</v>
       </c>
       <c r="AD21" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE21" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF21" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG21" s="2"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1984,43 +2116,48 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="2">
-        <v>5</v>
-      </c>
+      <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
+      <c r="P22" s="2">
+        <v>5</v>
+      </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-      <c r="W22" s="2">
-        <v>5</v>
-      </c>
+      <c r="W22" s="2"/>
       <c r="X22" s="2">
         <v>5</v>
       </c>
       <c r="Y22" s="2">
         <v>5</v>
       </c>
-      <c r="Z22" s="2">
-        <v>5</v>
-      </c>
-      <c r="AA22" s="2"/>
-      <c r="AB22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB22" s="2">
+        <v>5</v>
+      </c>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2">
+        <v>2</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -2028,124 +2165,144 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="2">
-        <v>5</v>
-      </c>
-      <c r="N23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2">
+        <v>5</v>
+      </c>
       <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
+      <c r="P23" s="2">
+        <v>5</v>
+      </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
-      <c r="V23" s="2">
-        <v>5</v>
-      </c>
+      <c r="V23" s="2"/>
       <c r="W23" s="2"/>
-      <c r="X23" s="2"/>
-      <c r="Y23" s="2"/>
-      <c r="Z23" s="2"/>
-      <c r="AA23" s="2"/>
-      <c r="AB23" s="2"/>
+      <c r="X23" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>5</v>
+      </c>
+      <c r="AA23" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB23" s="2">
+        <v>5</v>
+      </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2">
+        <v>3</v>
+      </c>
+      <c r="G24" s="2">
+        <v>3</v>
+      </c>
+      <c r="H24" s="2">
+        <v>3</v>
+      </c>
+      <c r="I24" s="2">
+        <v>3</v>
+      </c>
+      <c r="J24" s="2">
+        <v>3</v>
+      </c>
+      <c r="K24" s="2">
+        <v>3</v>
+      </c>
+      <c r="L24" s="2">
+        <v>3</v>
+      </c>
+      <c r="M24" s="2">
+        <v>3</v>
+      </c>
+      <c r="N24" s="2">
+        <v>3</v>
+      </c>
+      <c r="O24" s="2">
+        <v>3</v>
+      </c>
+      <c r="P24" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>3</v>
+      </c>
+      <c r="R24" s="2">
+        <v>3</v>
+      </c>
+      <c r="S24" s="2">
+        <v>3</v>
+      </c>
+      <c r="T24" s="2">
+        <v>3</v>
+      </c>
+      <c r="U24" s="2">
+        <v>3</v>
+      </c>
+      <c r="V24" s="2">
+        <v>3</v>
+      </c>
+      <c r="W24" s="2">
+        <v>3</v>
+      </c>
+      <c r="X24" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y24" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB24" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC24" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD24" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE24" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF24" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG24" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B24" s="2">
-        <v>3</v>
-      </c>
-      <c r="C24" s="2">
-        <v>3</v>
-      </c>
-      <c r="D24" s="2">
-        <v>3</v>
-      </c>
-      <c r="E24" s="2">
-        <v>3</v>
-      </c>
-      <c r="F24" s="2">
-        <v>3</v>
-      </c>
-      <c r="G24" s="2">
-        <v>3</v>
-      </c>
-      <c r="H24" s="2">
-        <v>3</v>
-      </c>
-      <c r="I24" s="2">
-        <v>3</v>
-      </c>
-      <c r="J24" s="2">
-        <v>3</v>
-      </c>
-      <c r="K24" s="2">
-        <v>3</v>
-      </c>
-      <c r="L24" s="2">
-        <v>3</v>
-      </c>
-      <c r="M24" s="2">
-        <v>5</v>
-      </c>
-      <c r="N24" s="2">
-        <v>3</v>
-      </c>
-      <c r="O24" s="2">
-        <v>3</v>
-      </c>
-      <c r="P24" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q24" s="2">
-        <v>3</v>
-      </c>
-      <c r="R24" s="2">
-        <v>3</v>
-      </c>
-      <c r="S24" s="2">
-        <v>3</v>
-      </c>
-      <c r="T24" s="2">
-        <v>3</v>
-      </c>
-      <c r="U24" s="2">
-        <v>3</v>
-      </c>
-      <c r="V24" s="2">
-        <v>3</v>
-      </c>
-      <c r="W24" s="2">
-        <v>3</v>
-      </c>
-      <c r="X24" s="2">
-        <v>3</v>
-      </c>
-      <c r="Y24" s="2">
-        <v>3</v>
-      </c>
-      <c r="Z24" s="2">
-        <v>3</v>
-      </c>
-      <c r="AA24" s="2">
-        <v>3</v>
-      </c>
-      <c r="AB24" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC24" s="2">
-        <v>3</v>
-      </c>
-      <c r="AD24" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2155,13 +2312,13 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2">
-        <v>5</v>
-      </c>
+      <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
+      <c r="N25" s="2">
+        <v>5</v>
+      </c>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
@@ -2178,10 +2335,13 @@
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
       <c r="AD25" s="2"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" s="2">
         <v>2</v>
@@ -2193,9 +2353,11 @@
         <v>2</v>
       </c>
       <c r="E26" s="2">
-        <v>3</v>
-      </c>
-      <c r="F26" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -2220,38 +2382,43 @@
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
       <c r="AD26" s="2"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="AC2:AG2"/>
+    <mergeCell ref="U3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="Q3:R4"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="X2:AB2"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="Q1:T1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="S3:T4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="N3:P4"/>
-    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="Q2:T2"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>